<commit_message>
Add all variants to Excel file
</commit_message>
<xml_diff>
--- a/results/MIC/Capreomycin.xlsx
+++ b/results/MIC/Capreomycin.xlsx
@@ -1533,7 +1533,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1581,14 +1581,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>tlyA_LoF</t>
+          <t>rrs_n.1401A&gt;G</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.257239622847246</v>
+        <v>1.100133497067009</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -1600,6 +1600,756 @@
         <v>1</v>
       </c>
       <c r="G2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>tlyA_LoF</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.257239622847246</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>tlyA_p.Gly232Asp</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.233324575737933</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>tlyA_p.Leu150Pro</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.1494490935172777</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.3166363636363636</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.957</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>rrs_n.513C&gt;T</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.09405252279081409</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.063</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.3290625</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.866</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>rrs_n.16T&gt;A</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.0925563190746522</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.0162</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.999</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>rrs_n.1402C&gt;T</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.0925563190746522</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.0162</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.999</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>rrs_n.514A&gt;C</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.0893499032312373</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.074</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.3525882352941176</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.855</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>rrs_n.239C&gt;A</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.08779545226084</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.091</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.37665</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.907</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>rrs_n.1322T&gt;G</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.0833744171202534</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.113</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.4026857142857142</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.885</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>rrs_n.1484G&gt;T</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.0816864935547125</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.124</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.4026857142857142</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.828</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>rrs_n.905C&gt;A</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.0704726450598086</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.149</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.4026857142857142</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.783</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>rrs_n.906A&gt;G</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.0646773331298814</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.143</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.4026857142857142</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.699</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>tlyA_p.Lys182Arg</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.0404872202860341</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.227</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.4134375</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.342</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>rrs_n.908A&gt;G</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.0308738698648582</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.226</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.4134375</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.296</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>tlyA_p.Gly196Arg</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.0146457195931928</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.299</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.4380845070422535</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.228</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>rrs_n.580T&gt;C</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.0133724024826514</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.4380845070422535</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.151</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>rrs_n.1180A&gt;G</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.0125532922599434</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.301</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.4380845070422535</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.224</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>rrs_n.236C&gt;G</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.0121107799976325</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.305</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.4380845070422535</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.242</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>rrs_n.365A&gt;G</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.0029572572673221</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.336</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.4380845070422535</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.07199999999999999</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.972</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>rrs_n.1064T&gt;C</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.0026278789266454</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.331</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.4380845070422535</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.091</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>rrs_n.492C&gt;T</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" t="n">
+        <v>-0.0154519329674277</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.376</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.4380845070422535</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.135</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>rrs_n.908A&gt;C</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" t="n">
+        <v>-0.0293170926510715</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.382</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.4380845070422535</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.324</v>
+      </c>
+      <c r="G24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>rrs_n.905C&gt;G</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" t="n">
+        <v>-0.0327385695579872</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.467</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.491</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.317</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>tlyA_p.Ter269Trpext*?</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" t="n">
+        <v>-0.034543126107123</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.324</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.4380845070422535</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.402</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>rrs_n.1107_1118dupTGTCTCATGTTG</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" t="n">
+        <v>-0.0417362318168323</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.466027397260274</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.357</v>
+      </c>
+      <c r="G27" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>rrs_n.-91C&gt;A</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" t="n">
+        <v>-0.0419411780965227</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.438</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.4794324324324324</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.342</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>rrs_n.-130T&gt;C</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" t="n">
+        <v>-0.0424888971450459</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.393</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.442125</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.408</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>rrs_n.1099G&gt;A</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" t="n">
+        <v>-0.0462660202312905</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.238</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.4134375</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.5580000000000001</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>rrs_n.514A&gt;T</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" t="n">
+        <v>-0.0504450247797895</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.233</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.4134375</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.5590000000000001</v>
+      </c>
+      <c r="G31" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>rrs_n.517C&gt;T</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" t="n">
+        <v>-0.0701813287501947</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.135</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.4026857142857142</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.718</v>
+      </c>
+      <c r="G32" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1614,7 +2364,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1662,23 +2412,23 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>tlyA_c.33A&gt;G</t>
+          <t>rrs_n.1401A&gt;G</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0677895641262804</v>
+        <v>1.100690621767613</v>
       </c>
       <c r="D2" t="n">
-        <v>0.136</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.3652571428571429</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.732</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
         <v>1</v>
@@ -1687,25 +2437,1075 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>tlyA_p.Gly232Asp</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.2321236815413161</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.094</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.998</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>tlyA_p.Leu150Pro</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.1486496120154856</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.026</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.329</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.974</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>tlyA_p.Gly138fs</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.1485166179467952</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.041</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.329</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.959</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>tlyA_p.Arg3*</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.1382217808691087</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.042</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.329</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.958</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>tlyA_p.Ser172fs</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.1381084258862389</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.034</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.329</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.966</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>tlyA_p.His68fs</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.1379811456756688</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.037</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.329</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.963</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>tlyA_p.Arg133fs</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.0983001935037819</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.093</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.3481481481481481</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.907</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>rrs_n.513C&gt;T</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.09816159330935111</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.068</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.3336999999999999</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.879</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>rrs_n.906A&gt;G</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.0959224361539929</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.07099999999999999</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.3336999999999999</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.871</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>rrs_n.1402C&gt;T</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.0924335429960341</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.094</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.996</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>rrs_n.16T&gt;A</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.0924335429960341</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.094</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.996</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>tlyA_p.Gly66fs</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.0904904783116373</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.097</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.3481481481481481</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.903</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>rrs_n.514A&gt;C</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.0891642682465028</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.079</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.3481481481481481</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.859</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>rrs_n.239C&gt;A</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.08672360946029729</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.08500000000000001</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.3481481481481481</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.909</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>rrs_n.1322T&gt;G</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.0845830510701879</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.3481481481481481</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.907</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>rrs_n.1484G&gt;T</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.0816464274515777</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.104</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.3491428571428571</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.848</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>rrs_n.905C&gt;A</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.0716432195825745</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.135</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.3652571428571429</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.797</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>tlyA_p.Lys226fs</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.0686004353219075</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.161</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.3982631578947369</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.725</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>tlyA_c.33A&gt;G</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.0677895641262804</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.136</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.3652571428571429</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.732</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>tlyA_p.His199fs</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.0565423855185428</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.3995</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.823</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>tlyA_p.Val198fs</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.0484550951935895</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.175</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.4012195121951219</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.596</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>tlyA_p.Lys182Arg</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.0400529117873419</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.205</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.4084727272727272</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.327</v>
+      </c>
+      <c r="G24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>tlyA_p.Ala215fs</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.0316105135989865</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.253</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.4116551724137931</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.352</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>rrs_n.908A&gt;G</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.0311962545426556</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.237</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.4084727272727272</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.294</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
           <t>tlyA_c.225G&gt;A</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="n">
+      <c r="B27" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" t="n">
         <v>0.0197701944483539</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D27" t="n">
         <v>0.312</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E27" t="n">
         <v>0.4164722222222222</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F27" t="n">
         <v>0.221</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G27" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>rrs_n.580T&gt;C</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.0151480268377733</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.356</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.423</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.182</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>tlyA_p.Gly196Arg</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.0138445241386908</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.279</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.4164722222222222</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.225</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>rrs_n.1180A&gt;G</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.0125435327405853</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.4164722222222222</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.217</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>tlyA_p.Arg60fs</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.0123274009610645</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.386</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.4394216867469879</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.135</v>
+      </c>
+      <c r="G31" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>rrs_n.236C&gt;G</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.0116668809131406</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.307</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.4164722222222222</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.228</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>rrs_n.365A&gt;G</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.0037941944086786</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.291</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.4164722222222222</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.102</v>
+      </c>
+      <c r="G33" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>rrs_n.1064T&gt;C</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.0035496999760696</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.345</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.423</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.095</v>
+      </c>
+      <c r="G34" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>rrs_n.908A&gt;C</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" t="n">
+        <v>-0.0279041290757351</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.423</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>tlyA_p.Gln21*</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" t="n">
+        <v>-0.0289611207985728</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.459</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.482</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.287</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>rrs_n.905C&gt;G</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" t="n">
+        <v>-0.0331860586946105</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.468</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.482</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.324</v>
+      </c>
+      <c r="G37" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>tlyA_p.Ter269Trpext*?</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" t="n">
+        <v>-0.0353876304185477</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.319</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.4164722222222222</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.415</v>
+      </c>
+      <c r="G38" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>rrs_n.492C&gt;T</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>1</v>
+      </c>
+      <c r="C39" t="n">
+        <v>-0.0377161421231084</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.316</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.4164722222222222</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.322</v>
+      </c>
+      <c r="G39" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>rrs_n.1107_1118dupTGTCTCATGTTG</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>1</v>
+      </c>
+      <c r="C40" t="n">
+        <v>-0.0409025410887591</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.471</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.482</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.345</v>
+      </c>
+      <c r="G40" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>rrs_n.-91C&gt;A</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" t="n">
+        <v>-0.0410850482415506</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.409</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.4523058823529411</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.399</v>
+      </c>
+      <c r="G41" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>rrs_n.-130T&gt;C</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>1</v>
+      </c>
+      <c r="C42" t="n">
+        <v>-0.0421977014952854</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.388</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.4394216867469879</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.438</v>
+      </c>
+      <c r="G42" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>rrs_n.1099G&gt;A</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>1</v>
+      </c>
+      <c r="C43" t="n">
+        <v>-0.0468893859125577</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.202</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.4084727272727272</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.595</v>
+      </c>
+      <c r="G43" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>rrs_n.514A&gt;T</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>1</v>
+      </c>
+      <c r="C44" t="n">
+        <v>-0.050748876648577</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.239</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.4084727272727272</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.569</v>
+      </c>
+      <c r="G44" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>rrs_n.517C&gt;T</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" t="n">
+        <v>-0.07045345709644921</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.131</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.3652571428571429</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.738</v>
+      </c>
+      <c r="G45" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>